<commit_message>
New engine model etc.
</commit_message>
<xml_diff>
--- a/TestData/Throttle vs LiterPerHour - Fixed RPM.xlsx
+++ b/TestData/Throttle vs LiterPerHour - Fixed RPM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>1k rpm Scania 730hp</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Tested gear 1 throughout 8, consistent resutlts</t>
+  </si>
+  <si>
+    <t>l/h 100%</t>
+  </si>
+  <si>
+    <t>&lt;factor for reading out digits in trendline</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,271 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.3330851055865849E-4"/>
+                  <c:y val="-3.0603019244457635E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>38.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="51365376"/>
+        <c:axId val="51366912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="51365376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51366912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="2.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="51366912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="40"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51365376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>l/h 100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -201,7 +471,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:f>Sheet1!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -209,117 +479,109 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3</c:v>
+                  <c:v>0.1640625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9</c:v>
+                  <c:v>0.20572916666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.1</c:v>
+                  <c:v>0.23697916666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.199999999999999</c:v>
+                  <c:v>0.265625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.3</c:v>
+                  <c:v>0.29427083333333337</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.2</c:v>
+                  <c:v>0.31770833333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.1</c:v>
+                  <c:v>0.3671875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.7</c:v>
+                  <c:v>0.40885416666666669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.2</c:v>
+                  <c:v>0.44791666666666669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.5</c:v>
+                  <c:v>0.48177083333333337</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.8</c:v>
+                  <c:v>0.515625</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>0.546875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.2</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.4</c:v>
+                  <c:v>0.609375</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.7</c:v>
+                  <c:v>0.64322916666666663</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26</c:v>
+                  <c:v>0.67708333333333337</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.5</c:v>
+                  <c:v>0.71614583333333337</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.4</c:v>
+                  <c:v>0.765625</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31.2</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>33.200000000000003</c:v>
+                  <c:v>0.86458333333333348</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>0.92968750000000011</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>38.4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="51473408"/>
-        <c:axId val="51444736"/>
+        <c:axId val="59982976"/>
+        <c:axId val="57650560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51473408"/>
+        <c:axId val="59982976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51444736"/>
+        <c:crossAx val="57650560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="2.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51444736"/>
+        <c:axId val="57650560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="40"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51473408"/>
+        <c:crossAx val="59982976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-        <c:minorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -346,10 +608,10 @@
       <xdr:rowOff>4969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33130</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>99390</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -363,6 +625,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>198782</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>480391</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -656,15 +948,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -674,11 +969,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -688,11 +986,15 @@
       <c r="C2">
         <v>1000</v>
       </c>
+      <c r="D2">
+        <f>B2/38.4*E$3</f>
+        <v>0</v>
+      </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -702,8 +1004,19 @@
       <c r="C3">
         <v>820</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="0">B3/38.4*E$3</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E3">
+        <f>POWER(10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>5</v>
       </c>
@@ -713,8 +1026,12 @@
       <c r="C4">
         <v>908</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>7.5</v>
       </c>
@@ -724,8 +1041,12 @@
       <c r="C5">
         <v>970</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.1640625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10</v>
       </c>
@@ -735,8 +1056,12 @@
       <c r="C6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.20572916666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>12.5</v>
       </c>
@@ -746,8 +1071,12 @@
       <c r="C7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.23697916666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>15</v>
       </c>
@@ -757,8 +1086,12 @@
       <c r="C8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.265625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>17.5</v>
       </c>
@@ -768,8 +1101,12 @@
       <c r="C9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.29427083333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>20</v>
       </c>
@@ -779,8 +1116,12 @@
       <c r="C10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.31770833333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>25</v>
       </c>
@@ -790,8 +1131,12 @@
       <c r="C11">
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.3671875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>30</v>
       </c>
@@ -801,8 +1146,12 @@
       <c r="C12">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.40885416666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>35</v>
       </c>
@@ -812,8 +1161,12 @@
       <c r="C13">
         <v>1000</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.44791666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>40</v>
       </c>
@@ -823,8 +1176,12 @@
       <c r="C14">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.48177083333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>45</v>
       </c>
@@ -834,8 +1191,12 @@
       <c r="C15">
         <v>1000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.515625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>50</v>
       </c>
@@ -845,8 +1206,12 @@
       <c r="C16">
         <v>1000</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.546875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>55</v>
       </c>
@@ -856,8 +1221,12 @@
       <c r="C17">
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.578125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>60</v>
       </c>
@@ -867,8 +1236,12 @@
       <c r="C18">
         <v>1000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.609375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>65</v>
       </c>
@@ -878,8 +1251,12 @@
       <c r="C19">
         <v>1000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.64322916666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>70</v>
       </c>
@@ -889,8 +1266,12 @@
       <c r="C20">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.67708333333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>75</v>
       </c>
@@ -900,8 +1281,12 @@
       <c r="C21">
         <v>1000</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.71614583333333337</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>80</v>
       </c>
@@ -911,8 +1296,12 @@
       <c r="C22">
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.765625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>85</v>
       </c>
@@ -922,8 +1311,12 @@
       <c r="C23">
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>90</v>
       </c>
@@ -933,8 +1326,12 @@
       <c r="C24">
         <v>1000</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.86458333333333348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>95</v>
       </c>
@@ -944,8 +1341,12 @@
       <c r="C25">
         <v>1000</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.92968750000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>100</v>
       </c>
@@ -954,6 +1355,10 @@
       </c>
       <c r="C26">
         <v>1000</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>